<commit_message>
Updated Exam Spreadsheet to include instructions
</commit_message>
<xml_diff>
--- a/public/DecaExam.xlsx
+++ b/public/DecaExam.xlsx
@@ -5,16 +5,18 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maanav\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maanav\Desktop\turnerfentondecanode\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" tabRatio="763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Exam 1" sheetId="17" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="18" r:id="rId1"/>
+    <sheet name="Exam 1" sheetId="17" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Right</t>
   </si>
@@ -61,12 +63,72 @@
   <si>
     <t>To Review</t>
   </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>1. Acquire an Exam Document (of your choice) with answers</t>
+  </si>
+  <si>
+    <t>2. Write your answer in the "Answer + Notes" column. Add notes as much as you need for revision</t>
+  </si>
+  <si>
+    <t>Ensure that the first letter in this area is your answer for the tool to work successfully:</t>
+  </si>
+  <si>
+    <t>For Example: A but I think B could be the answer</t>
+  </si>
+  <si>
+    <t>3. Go through the whole exam, only using the "Answer + Notes" column, matching questions to the "Question #"</t>
+  </si>
+  <si>
+    <t>4. When you're done, go through the answers and input the correct answer in the "Paste answers here" area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Congratulations! You've done it. </t>
+  </si>
+  <si>
+    <t>You should see an in depth analysis of the questions you were:</t>
+  </si>
+  <si>
+    <t>The amount of Notes you made</t>
+  </si>
+  <si>
+    <t>This count is regardless of right/wrong</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A or B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Wrong or unsure questions</t>
+  </si>
+  <si>
+    <t>Unsure are any questions with notes</t>
+  </si>
+  <si>
+    <t>In my opinon, the orange section is the most insightful, and I call it the "uncertainty percentage"</t>
+  </si>
+  <si>
+    <t>This might be the most useful area since over time it should measure your changes in confidence about exams!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,8 +166,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +210,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -155,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -174,6 +248,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,11 +562,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F31B5D-E9B7-4CC0-B588-CAB78549F014}">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -550,14 +725,16 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="C3" s="4" t="str">
         <f t="shared" ref="C3:C66" si="0">UPPER(CONCATENATE(LEFT(B3,1)))</f>
-        <v/>
+        <v>A</v>
       </c>
       <c r="D3" s="4" t="str">
         <f t="shared" ref="D3:D66" si="1">CONCATENATE(LEFT(N3,1))</f>
-        <v/>
+        <v>A</v>
       </c>
       <c r="E3">
         <f>IF(C3=D3,1,0)</f>
@@ -565,33 +742,38 @@
       </c>
       <c r="F3" s="6">
         <f>IF(LEN(B3)&lt;2, 0, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f>IF(E3=0,1,IF(SUM(E3:F3)=2,1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="5">
         <f>SUM(E3:E102)</f>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M3" s="10"/>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="C4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>B</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>B</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E67" si="2">IF(C4=D4,1,0)</f>
@@ -610,26 +792,31 @@
       </c>
       <c r="J4" s="5">
         <f>100-J3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="10"/>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="C5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>D</v>
       </c>
       <c r="D5" s="4" t="str">
         <f>CONCATENATE(LEFT(N5,1))</f>
-        <v/>
+        <v>C</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" si="3"/>
@@ -637,16 +824,19 @@
       </c>
       <c r="G5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="5">
         <f>SUM(F3:F102)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="10"/>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -678,7 +868,7 @@
       </c>
       <c r="J6" s="5">
         <f>SUM(G3:G102)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M6" s="10"/>
     </row>

</xml_diff>